<commit_message>
Updated hw3.cpp to include false.positive funciton and  kahan.b and kahan.c equations, fmsroot1d.h to include the secant function which is used in the false.positive function, and the hw3.xlsx file to show the roots using the false.poistive method for whatever selected function and starting bracket is entered.
</commit_message>
<xml_diff>
--- a/hw3.xlsx
+++ b/hw3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal2222\source\repos\xlladdins\xllfloat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\source\repos\xllfloat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EDB811-34F1-462D-A5B0-66E0DF56563B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B084AB9E-97BE-4D36-92F3-8F0BEFBA177A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5C1C8244-EF68-49EF-BEC5-ED8ACE692021}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1C8244-EF68-49EF-BEC5-ED8ACE692021}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -258,304 +258,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0101010101010102</c:v>
+                  <c:v>0.10404040404040404</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0202020202020201</c:v>
+                  <c:v>0.10808080808080808</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0303030303030303</c:v>
+                  <c:v>0.11212121212121212</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0404040404040404</c:v>
+                  <c:v>0.11616161616161616</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0505050505050506</c:v>
+                  <c:v>0.1202020202020202</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0606060606060606</c:v>
+                  <c:v>0.12424242424242425</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0707070707070707</c:v>
+                  <c:v>0.12828282828282828</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0808080808080809</c:v>
+                  <c:v>0.13232323232323234</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0909090909090908</c:v>
+                  <c:v>0.13636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.101010101010101</c:v>
+                  <c:v>0.14040404040404042</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1111111111111112</c:v>
+                  <c:v>0.14444444444444446</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1212121212121211</c:v>
+                  <c:v>0.1484848484848485</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1313131313131313</c:v>
+                  <c:v>0.15252525252525254</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.1414141414141414</c:v>
+                  <c:v>0.15656565656565657</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1515151515151516</c:v>
+                  <c:v>0.16060606060606061</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1616161616161615</c:v>
+                  <c:v>0.16464646464646465</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.1717171717171717</c:v>
+                  <c:v>0.16868686868686869</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.1818181818181819</c:v>
+                  <c:v>0.17272727272727273</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.191919191919192</c:v>
+                  <c:v>0.17676767676767677</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.202020202020202</c:v>
+                  <c:v>0.18080808080808081</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2121212121212122</c:v>
+                  <c:v>0.18484848484848487</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.2222222222222223</c:v>
+                  <c:v>0.18888888888888888</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.2323232323232323</c:v>
+                  <c:v>0.19292929292929295</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.2424242424242424</c:v>
+                  <c:v>0.19696969696969696</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2525252525252526</c:v>
+                  <c:v>0.20101010101010103</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.2626262626262625</c:v>
+                  <c:v>0.20505050505050504</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.2727272727272727</c:v>
+                  <c:v>0.20909090909090911</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.2828282828282829</c:v>
+                  <c:v>0.21313131313131314</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2929292929292928</c:v>
+                  <c:v>0.21717171717171718</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.303030303030303</c:v>
+                  <c:v>0.22121212121212122</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.3131313131313131</c:v>
+                  <c:v>0.22525252525252526</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.3232323232323233</c:v>
+                  <c:v>0.2292929292929293</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.3333333333333335</c:v>
+                  <c:v>0.23333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.3434343434343434</c:v>
+                  <c:v>0.23737373737373738</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.3535353535353536</c:v>
+                  <c:v>0.24141414141414141</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.3636363636363638</c:v>
+                  <c:v>0.24545454545454545</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.3737373737373737</c:v>
+                  <c:v>0.24949494949494949</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.3838383838383839</c:v>
+                  <c:v>0.2535353535353535</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.393939393939394</c:v>
+                  <c:v>0.25757575757575757</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.404040404040404</c:v>
+                  <c:v>0.26161616161616164</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.4141414141414141</c:v>
+                  <c:v>0.2656565656565657</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.4242424242424243</c:v>
+                  <c:v>0.26969696969696971</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.4343434343434343</c:v>
+                  <c:v>0.27373737373737372</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.4444444444444444</c:v>
+                  <c:v>0.27777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.4545454545454546</c:v>
+                  <c:v>0.28181818181818186</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.4646464646464648</c:v>
+                  <c:v>0.28585858585858587</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.4747474747474749</c:v>
+                  <c:v>0.28989898989898988</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.4848484848484849</c:v>
+                  <c:v>0.29393939393939394</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.494949494949495</c:v>
+                  <c:v>0.29797979797979801</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.5050505050505052</c:v>
+                  <c:v>0.30202020202020202</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.5151515151515151</c:v>
+                  <c:v>0.30606060606060603</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.5252525252525253</c:v>
+                  <c:v>0.3101010101010101</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.5353535353535355</c:v>
+                  <c:v>0.31414141414141417</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.5454545454545454</c:v>
+                  <c:v>0.31818181818181818</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.5555555555555556</c:v>
+                  <c:v>0.32222222222222219</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.5656565656565657</c:v>
+                  <c:v>0.32626262626262625</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.5757575757575757</c:v>
+                  <c:v>0.33030303030303032</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.5858585858585859</c:v>
+                  <c:v>0.33434343434343439</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.595959595959596</c:v>
+                  <c:v>0.3383838383838384</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.606060606060606</c:v>
+                  <c:v>0.34242424242424241</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.6161616161616164</c:v>
+                  <c:v>0.34646464646464648</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.6262626262626263</c:v>
+                  <c:v>0.35050505050505054</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.6363636363636365</c:v>
+                  <c:v>0.3545454545454545</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.6464646464646466</c:v>
+                  <c:v>0.35858585858585856</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.6565656565656566</c:v>
+                  <c:v>0.36262626262626263</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.6666666666666667</c:v>
+                  <c:v>0.3666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.6767676767676769</c:v>
+                  <c:v>0.37070707070707076</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.6868686868686869</c:v>
+                  <c:v>0.37474747474747472</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.696969696969697</c:v>
+                  <c:v>0.37878787878787878</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.7070707070707072</c:v>
+                  <c:v>0.38282828282828285</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.7171717171717171</c:v>
+                  <c:v>0.38686868686868692</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.7272727272727273</c:v>
+                  <c:v>0.39090909090909087</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.7373737373737375</c:v>
+                  <c:v>0.39494949494949494</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.7474747474747474</c:v>
+                  <c:v>0.39898989898989901</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.7575757575757578</c:v>
+                  <c:v>0.40303030303030307</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.7676767676767677</c:v>
+                  <c:v>0.40707070707070703</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.7777777777777777</c:v>
+                  <c:v>0.41111111111111109</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.7878787878787881</c:v>
+                  <c:v>0.41515151515151516</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.797979797979798</c:v>
+                  <c:v>0.41919191919191923</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.8080808080808082</c:v>
+                  <c:v>0.42323232323232318</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.8181818181818183</c:v>
+                  <c:v>0.42727272727272725</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.8282828282828283</c:v>
+                  <c:v>0.43131313131313131</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.8383838383838385</c:v>
+                  <c:v>0.43535353535353538</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.8484848484848486</c:v>
+                  <c:v>0.43939393939393945</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.8585858585858586</c:v>
+                  <c:v>0.4434343434343434</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.8686868686868687</c:v>
+                  <c:v>0.44747474747474747</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.8787878787878789</c:v>
+                  <c:v>0.45151515151515154</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.8888888888888888</c:v>
+                  <c:v>0.4555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.8989898989898992</c:v>
+                  <c:v>0.45959595959595956</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.9090909090909092</c:v>
+                  <c:v>0.46363636363636362</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.9191919191919191</c:v>
+                  <c:v>0.46767676767676769</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.9292929292929295</c:v>
+                  <c:v>0.47171717171717176</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.9393939393939394</c:v>
+                  <c:v>0.47575757575757571</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.9494949494949496</c:v>
+                  <c:v>0.47979797979797978</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.9595959595959598</c:v>
+                  <c:v>0.48383838383838385</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.9696969696969697</c:v>
+                  <c:v>0.48787878787878791</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.9797979797979799</c:v>
+                  <c:v>0.49191919191919198</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.9898989898989901</c:v>
+                  <c:v>0.49595959595959593</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -567,304 +567,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>-0.51099230432308951</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0195857049208437</c:v>
+                  <c:v>-0.47140419921131316</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.037922164594459</c:v>
+                  <c:v>-0.43332708520626406</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0549842696098644</c:v>
+                  <c:v>-0.39665021591742999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0707466607111975</c:v>
+                  <c:v>-0.36127461786849341</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0851837287977073</c:v>
+                  <c:v>-0.32711147968537158</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0982696149237601</c:v>
+                  <c:v>-0.2940808076936261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1099782102988325</c:v>
+                  <c:v>-0.26211029674067837</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1202831562875222</c:v>
+                  <c:v>-0.23113437617613841</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1291578444095345</c:v>
+                  <c:v>-0.20109339936436621</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.1365754163396948</c:v>
+                  <c:v>-0.17193295157117347</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.1425087639079408</c:v>
+                  <c:v>-0.14360325606551605</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.1469305290993246</c:v>
+                  <c:v>-0.11605866217200039</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1498131040540134</c:v>
+                  <c:v>-8.9257202068035973E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.151128631067289</c:v>
+                  <c:v>-6.3160205537478142E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.150849002589549</c:v>
+                  <c:v>-3.7731963817539203E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.1489458612263022</c:v>
+                  <c:v>-1.2939435217864335E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.1453905997381773</c:v>
+                  <c:v>1.1248013566421961E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.1401543610409126</c:v>
+                  <c:v>3.4858835518448282E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.133208038205364</c:v>
+                  <c:v>5.7919504989836897E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.124522274457501</c:v>
+                  <c:v>8.0454696594655428E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.114067463178408</c:v>
+                  <c:v>0.10248744433071234</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.1018137479042824</c:v>
+                  <c:v>0.12403928349404224</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.0877310223264409</c:v>
+                  <c:v>0.14513037757217709</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.0717889302913104</c:v>
+                  <c:v>0.16577963198461465</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.0539568658004317</c:v>
+                  <c:v>0.18600479627327429</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.0342039730104648</c:v>
+                  <c:v>0.20582255612236389</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0124991462331812</c:v>
+                  <c:v>0.22524861639865201</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.9888110299354667</c:v>
+                  <c:v>0.24429777624351084</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.9631080187393248</c:v>
+                  <c:v>0.26298399711250481</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.9353582574218695</c:v>
+                  <c:v>0.28132046454267046</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.9055296409153311</c:v>
+                  <c:v>0.29931964432878305</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.8735898143070564</c:v>
+                  <c:v>0.31699333370508936</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.8395061728395046</c:v>
+                  <c:v>0.33435270805604783</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.8032458619102529</c:v>
+                  <c:v>0.3514083636166862</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.7647757770719856</c:v>
+                  <c:v>0.36817035656875413</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.7240625640325113</c:v>
+                  <c:v>0.38464823889165689</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.6810726186547456</c:v>
+                  <c:v>0.40085109128610991</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.6357720869567212</c:v>
+                  <c:v>0.41678755345270524</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.5881268651115867</c:v>
+                  <c:v>0.43246585197634096</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.5381025994476083</c:v>
+                  <c:v>0.44789382604011518</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.485664686448156</c:v>
+                  <c:v>0.46307895116830255</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.4307782727517271</c:v>
+                  <c:v>0.47802836117692737</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.373408255151924</c:v>
+                  <c:v>0.49274886849187155</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.31351928059747</c:v>
+                  <c:v>0.50724698297803839</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.2510757461921989</c:v>
+                  <c:v>0.52152892940859641</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.1860417991950643</c:v>
+                  <c:v>0.53560066369045878</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.1183813370201268</c:v>
+                  <c:v>0.54946788795074508</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.0480580072365706</c:v>
+                  <c:v>0.5631360645788217</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.9750352075686841</c:v>
+                  <c:v>0.57661042930947415</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.8992760858958793</c:v>
+                  <c:v>0.58989600342470205</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.8207435402526801</c:v>
+                  <c:v>0.60299760514441392</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.7394002188287248</c:v>
+                  <c:v>0.61591986026984724</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.6552085199687632</c:v>
+                  <c:v>0.62866721213775667</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.5681305921726674</c:v>
+                  <c:v>0.64124393093822074</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.4781283340954126</c:v>
+                  <c:v>0.65365412244424481</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.3851633945470994</c:v>
+                  <c:v>0.66590173619713888</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.2891971724929396</c:v>
+                  <c:v>0.67799057318785705</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.1901908170532591</c:v>
+                  <c:v>0.68992429307106884</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.0881052275034948</c:v>
+                  <c:v>0.7017064209456334</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.9829010532742082</c:v>
+                  <c:v>0.71334035373235738</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.8745386939510595</c:v>
+                  <c:v>0.72482936617737603</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.7629782992748426</c:v>
+                  <c:v>0.73617661650719812</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.6481797691414508</c:v>
+                  <c:v>0.74738515175936715</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.5301027536018985</c:v>
+                  <c:v>0.75845791281079178</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.4087066528623202</c:v>
+                  <c:v>0.76939773912406118</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.2839506172839492</c:v>
+                  <c:v>0.78020737323049849</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.1557935473831495</c:v>
+                  <c:v>0.79088946496725276</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.024194093831392</c:v>
+                  <c:v>0.80144657548442799</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.88911065745525875</c:v>
+                  <c:v>0.81188118103703832</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.75050138923645626</c:v>
+                  <c:v>0.82219567657548431</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.60832419031180507</c:v>
+                  <c:v>0.83239237914724074</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.46253671197322532</c:v>
+                  <c:v>0.84247353112151502</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.31309635566776883</c:v>
+                  <c:v>0.85244130324780032</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.15996027299759596</c:v>
+                  <c:v>0.86229779755845748</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>3.0853657199720885E-3</c:v>
+                  <c:v>0.87204505012475164</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-0.15757171425269867</c:v>
+                  <c:v>0.88168503367511353</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-0.32205456485291784</c:v>
+                  <c:v>0.89121966008377951</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-0.4904070338580766</c:v>
+                  <c:v>0.90065078273741606</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-0.66267321889042563</c:v>
+                  <c:v>0.90998019878681191</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-0.83889746741713189</c:v>
+                  <c:v>0.91920965129024945</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-1.0191243767502254</c:v>
+                  <c:v>0.92834083125472577</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-1.2033987940466258</c:v>
+                  <c:v>0.93737537958078287</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-1.3917658163081494</c:v>
+                  <c:v>0.94631488891634141</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-1.5842707903814865</c:v>
+                  <c:v>0.955160905424569</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>-1.7809593129582115</c:v>
+                  <c:v>0.9639149304705058</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>-1.9818772305747974</c:v>
+                  <c:v>0.97257842223085889</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>-2.1870706396125907</c:v>
+                  <c:v>0.98115279723110416</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>-2.3965858862978209</c:v>
+                  <c:v>0.98963943181377878</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>-2.6104695667016209</c:v>
+                  <c:v>0.99803966354160234</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>-2.828768526739978</c:v>
+                  <c:v>1.0063547925388427</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>-3.0515298621737958</c:v>
+                  <c:v>1.014586082774138</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>-3.2788009186088587</c:v>
+                  <c:v>1.0227347632877895</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>-3.5106292914958086</c:v>
+                  <c:v>1.0308020293663602</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>-3.7470628261302092</c:v>
+                  <c:v>1.0387890436672522</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>-3.9881496176524873</c:v>
+                  <c:v>1.0466969372957633</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>-4.2339380110479539</c:v>
+                  <c:v>1.0545268108370003</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>-4.4844766011468256</c:v>
+                  <c:v>1.0622797353448683</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>-4.7398142326241839</c:v>
+                  <c:v>1.0699567532902383</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>-5</c:v>
+                  <c:v>1.0775588794702773</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1960,64 +1960,64 @@
   <dimension ref="B2:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" customWidth="1"/>
-    <col min="13" max="13" width="3.59765625" customWidth="1"/>
+    <col min="7" max="7" width="3.5546875" customWidth="1"/>
+    <col min="13" max="13" width="3.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f t="array" ref="C2">_xll.KAHAN.A</f>
-        <v>-1412235196</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
+        <f t="array" ref="C2">_xll.KAHAN.C</f>
+        <v>1913454664</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D3" cm="1">
         <f t="array" ref="D3">_xll.XLL.UDF(function,C3)</f>
-        <v>4</v>
+        <v>-0.51099230432308951</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D4" cm="1">
         <f t="array" ref="D4">_xll.XLL.UDF(function,C4)</f>
-        <v>-5</v>
+        <v>1.0775588794702773</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="N5" cm="1">
         <f t="array" ref="N5">_xll.ARRAY.SET(_xll.ARRAY.INTERVAL($C$3,$C$4,100))</f>
-        <v>-412506</v>
+        <v>212736</v>
       </c>
       <c r="O5" cm="1">
         <f t="array" ref="O5">_xll.ARRAY.SET(_xll.ARRAY.APPLY(function,_xll.ARRAY.GET(N5)))</f>
-        <v>-412316</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
+        <v>212832</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2044,877 +2044,1619 @@
       </c>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C7" cm="1">
         <f t="array" ref="C7:D7">_xll.BISECT(function,C3,C4)</f>
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="E7">
         <f>D7-C7</f>
-        <v>0.5</v>
+        <v>0.19999999999999998</v>
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">_xll.XLL.UDF(function,C7)</f>
-        <v>2.9375</v>
+        <v>-0.51099230432308951</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I7" cm="1">
+        <f t="array" ref="I7:J7">_xll.FALSE.POSITIVE(function,C3,C4)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J7">
+        <v>0.22866876674451747</v>
+      </c>
       <c r="K7">
         <f>J7-I7</f>
-        <v>0</v>
+        <v>0.12866876674451747</v>
       </c>
       <c r="L7" cm="1">
         <f t="array" ref="L7">_xll.XLL.UDF(function,I7)</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C8" cm="1">
         <f t="array" ref="C8:D8">_xll.BISECT(function,C7,D7)</f>
-        <v>1.75</v>
+        <v>0.1</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:E57" si="0">D8-C8</f>
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">_xll.XLL.UDF(function,C8)</f>
-        <v>0.12109375</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-0.51099230432308951</v>
+      </c>
+      <c r="I8" cm="1">
+        <f t="array" ref="I8:J8">_xll.FALSE.POSITIVE(function,I7,J7)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J8">
+        <v>0.17966878158094995</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8:K57" si="1">J8-I8</f>
+        <v>7.9668781580949949E-2</v>
+      </c>
+      <c r="L8" cm="1">
+        <f t="array" ref="L8">_xll.XLL.UDF(function,I8)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C9" cm="1">
         <f t="array" ref="C9:D9">_xll.BISECT(function,C8,D8)</f>
-        <v>1.75</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="D9">
-        <v>1.875</v>
+        <v>0.2</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>4.9999999999999989E-2</v>
       </c>
       <c r="F9" cm="1">
         <f t="array" ref="F9">_xll.XLL.UDF(function,C9)</f>
-        <v>0.12109375</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-0.10592317392030241</v>
+      </c>
+      <c r="I9" cm="1">
+        <f t="array" ref="I9:J9">_xll.FALSE.POSITIVE(function,I8,J8)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J9">
+        <v>0.16957279561756278</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>6.9572795617562772E-2</v>
+      </c>
+      <c r="L9" cm="1">
+        <f t="array" ref="L9">_xll.XLL.UDF(function,I9)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C10" cm="1">
         <f t="array" ref="C10:D10">_xll.BISECT(function,C9,D9)</f>
-        <v>1.75</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="D10">
-        <v>1.8125</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>2.4999999999999994E-2</v>
       </c>
       <c r="F10" cm="1">
         <f t="array" ref="F10">_xll.XLL.UDF(function,C10)</f>
-        <v>0.12109375</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-0.10592317392030241</v>
+      </c>
+      <c r="I10" cm="1">
+        <f t="array" ref="I10:J10">_xll.FALSE.POSITIVE(function,I9,J9)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J10">
+        <v>0.16739994031542887</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>6.7399940315428869E-2</v>
+      </c>
+      <c r="L10" cm="1">
+        <f t="array" ref="L10">_xll.XLL.UDF(function,I10)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C11" cm="1">
         <f t="array" ref="C11:D11">_xll.BISECT(function,C10,D10)</f>
-        <v>1.75</v>
+        <v>0.16250000000000003</v>
       </c>
       <c r="D11">
-        <v>1.78125</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>1.2499999999999983E-2</v>
       </c>
       <c r="F11" cm="1">
         <f t="array" ref="F11">_xll.XLL.UDF(function,C11)</f>
-        <v>0.12109375</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-2.6033233110659918E-2</v>
+      </c>
+      <c r="I11" cm="1">
+        <f t="array" ref="I11:J11">_xll.FALSE.POSITIVE(function,I10,J10)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J11">
+        <v>0.16692740062941941</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>6.6927400629419403E-2</v>
+      </c>
+      <c r="L11" cm="1">
+        <f t="array" ref="L11">_xll.XLL.UDF(function,I11)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C12" cm="1">
         <f t="array" ref="C12:D12">_xll.BISECT(function,C11,D11)</f>
-        <v>1.75</v>
+        <v>0.16250000000000003</v>
       </c>
       <c r="D12">
-        <v>1.765625</v>
+        <v>0.16875000000000001</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>1.5625E-2</v>
+        <v>6.2499999999999778E-3</v>
       </c>
       <c r="F12" cm="1">
         <f t="array" ref="F12">_xll.XLL.UDF(function,C12)</f>
-        <v>0.12109375</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-2.6033233110659918E-2</v>
+      </c>
+      <c r="I12" cm="1">
+        <f t="array" ref="I12:J12">_xll.FALSE.POSITIVE(function,I11,J11)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J12">
+        <v>0.16682439681438094</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>6.6824396814380932E-2</v>
+      </c>
+      <c r="L12" cm="1">
+        <f t="array" ref="L12">_xll.XLL.UDF(function,I12)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C13" cm="1">
         <f t="array" ref="C13:D13">_xll.BISECT(function,C12,D12)</f>
-        <v>1.75</v>
+        <v>0.16562500000000002</v>
       </c>
       <c r="D13">
-        <v>1.7578125</v>
+        <v>0.16875000000000001</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>7.8125E-3</v>
+        <v>3.1249999999999889E-3</v>
       </c>
       <c r="F13" cm="1">
         <f t="array" ref="F13">_xll.XLL.UDF(function,C13)</f>
-        <v>0.12109375</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-7.0271274349637119E-3</v>
+      </c>
+      <c r="I13" cm="1">
+        <f t="array" ref="I13:J13">_xll.FALSE.POSITIVE(function,I12,J12)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J13">
+        <v>0.16680193271097565</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>6.6801932710975648E-2</v>
+      </c>
+      <c r="L13" cm="1">
+        <f t="array" ref="L13">_xll.XLL.UDF(function,I13)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C14" cm="1">
         <f t="array" ref="C14:D14">_xll.BISECT(function,C13,D13)</f>
-        <v>1.75390625</v>
+        <v>0.16562500000000002</v>
       </c>
       <c r="D14">
-        <v>1.7578125</v>
+        <v>0.16718750000000002</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>3.90625E-3</v>
+        <v>1.5624999999999944E-3</v>
       </c>
       <c r="F14" cm="1">
         <f t="array" ref="F14">_xll.XLL.UDF(function,C14)</f>
-        <v>6.0510217910632491E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-7.0271274349637119E-3</v>
+      </c>
+      <c r="I14" cm="1">
+        <f t="array" ref="I14:J14">_xll.FALSE.POSITIVE(function,I13,J13)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J14">
+        <v>0.166797032970606</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>6.6797032970605991E-2</v>
+      </c>
+      <c r="L14" cm="1">
+        <f t="array" ref="L14">_xll.XLL.UDF(function,I14)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C15" cm="1">
         <f t="array" ref="C15:D15">_xll.BISECT(function,C14,D14)</f>
-        <v>1.755859375</v>
+        <v>0.16640625000000003</v>
       </c>
       <c r="D15">
-        <v>1.7578125</v>
+        <v>0.16718750000000002</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1.953125E-3</v>
+        <v>7.8124999999998335E-4</v>
       </c>
       <c r="F15" cm="1">
         <f t="array" ref="F15">_xll.XLL.UDF(function,C15)</f>
-        <v>3.0007383538759314E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-2.3320107229970566E-3</v>
+      </c>
+      <c r="I15" cm="1">
+        <f t="array" ref="I15:J15">_xll.FALSE.POSITIVE(function,I14,J14)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J15">
+        <v>0.1667959642416853</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>6.6795964241685296E-2</v>
+      </c>
+      <c r="L15" cm="1">
+        <f t="array" ref="L15">_xll.XLL.UDF(function,I15)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C16" cm="1">
         <f t="array" ref="C16:D16">_xll.BISECT(function,C15,D15)</f>
-        <v>1.7568359375</v>
+        <v>0.16640625000000003</v>
       </c>
       <c r="D16">
-        <v>1.7578125</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>9.765625E-4</v>
+        <v>3.906249999999778E-4</v>
       </c>
       <c r="F16" cm="1">
         <f t="array" ref="F16">_xll.XLL.UDF(function,C16)</f>
-        <v>1.4703062041917292E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.3320107229970566E-3</v>
+      </c>
+      <c r="I16" cm="1">
+        <f t="array" ref="I16:J16">_xll.FALSE.POSITIVE(function,I15,J15)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J16">
+        <v>0.16679573112983606</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>6.6795731129836056E-2</v>
+      </c>
+      <c r="L16" cm="1">
+        <f t="array" ref="L16">_xll.XLL.UDF(function,I16)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" cm="1">
         <f t="array" ref="C17:D17">_xll.BISECT(function,C16,D16)</f>
-        <v>1.75732421875</v>
+        <v>0.16660156250000002</v>
       </c>
       <c r="D17">
-        <v>1.7578125</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>4.8828125E-4</v>
+        <v>1.953124999999889E-4</v>
       </c>
       <c r="F17" cm="1">
         <f t="array" ref="F17">_xll.XLL.UDF(function,C17)</f>
-        <v>7.0376580442257364E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.1616995234697695E-3</v>
+      </c>
+      <c r="I17" cm="1">
+        <f t="array" ref="I17:J17">_xll.FALSE.POSITIVE(function,I16,J16)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J17">
+        <v>0.16679568028326885</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>6.6795680283268849E-2</v>
+      </c>
+      <c r="L17" cm="1">
+        <f t="array" ref="L17">_xll.XLL.UDF(function,I17)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" cm="1">
         <f t="array" ref="C18:D18">_xll.BISECT(function,C17,D17)</f>
-        <v>1.757568359375</v>
+        <v>0.16669921875000002</v>
       </c>
       <c r="D18">
-        <v>1.7578125</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>2.44140625E-4</v>
+        <v>9.7656249999994449E-5</v>
       </c>
       <c r="F18" cm="1">
         <f t="array" ref="F18">_xll.XLL.UDF(function,C18)</f>
-        <v>3.2016430855001943E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-5.7706189945448271E-4</v>
+      </c>
+      <c r="I18" cm="1">
+        <f t="array" ref="I18:J18">_xll.FALSE.POSITIVE(function,I17,J17)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J18">
+        <v>0.16679566919256689</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>6.6795669192566881E-2</v>
+      </c>
+      <c r="L18" cm="1">
+        <f t="array" ref="L18">_xll.XLL.UDF(function,I18)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" cm="1">
         <f t="array" ref="C19:D19">_xll.BISECT(function,C18,D18)</f>
-        <v>1.7576904296875</v>
+        <v>0.166748046875</v>
       </c>
       <c r="D19">
-        <v>1.7578125</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>1.220703125E-4</v>
+        <v>4.8828125000011102E-5</v>
       </c>
       <c r="F19" cm="1">
         <f t="array" ref="F19">_xll.XLL.UDF(function,C19)</f>
-        <v>1.2828070976524941E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.8487240560673974E-4</v>
+      </c>
+      <c r="I19" cm="1">
+        <f t="array" ref="I19:J19">_xll.FALSE.POSITIVE(function,I18,J18)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J19">
+        <v>0.16679566677345226</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>6.679566677345225E-2</v>
+      </c>
+      <c r="L19" cm="1">
+        <f t="array" ref="L19">_xll.XLL.UDF(function,I19)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" cm="1">
         <f t="array" ref="C20:D20">_xll.BISECT(function,C19,D19)</f>
-        <v>1.75775146484375</v>
+        <v>0.16677246093750001</v>
       </c>
       <c r="D20">
-        <v>1.7578125</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>6.103515625E-5</v>
+        <v>2.4414062500005551E-5</v>
       </c>
       <c r="F20" cm="1">
         <f t="array" ref="F20">_xll.XLL.UDF(function,C20)</f>
-        <v>3.2318194303826431E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.3880996628686784E-4</v>
+      </c>
+      <c r="I20" cm="1">
+        <f t="array" ref="I20:J20">_xll.FALSE.POSITIVE(function,I19,J19)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J20">
+        <v>0.16679566624579262</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>6.6795666245792612E-2</v>
+      </c>
+      <c r="L20" cm="1">
+        <f t="array" ref="L20">_xll.XLL.UDF(function,I20)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" cm="1">
         <f t="array" ref="C21:D21">_xll.BISECT(function,C20,D20)</f>
-        <v>1.75775146484375</v>
+        <v>0.16678466796875002</v>
       </c>
       <c r="D21">
-        <v>1.757781982421875</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>3.0517578125E-5</v>
+        <v>1.2207031249988898E-5</v>
       </c>
       <c r="F21" cm="1">
         <f t="array" ref="F21">_xll.XLL.UDF(function,C21)</f>
-        <v>3.2318194303826431E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-6.5786820788225862E-5</v>
+      </c>
+      <c r="I21" cm="1">
+        <f t="array" ref="I21:J21">_xll.FALSE.POSITIVE(function,I20,J20)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J21">
+        <v>0.16679566613069896</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>6.6795666130698955E-2</v>
+      </c>
+      <c r="L21" cm="1">
+        <f t="array" ref="L21">_xll.XLL.UDF(function,I21)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
         <f t="array" ref="C22:D22">_xll.BISECT(function,C21,D21)</f>
-        <v>1.7577667236328125</v>
+        <v>0.16679077148437502</v>
       </c>
       <c r="D22">
-        <v>1.757781982421875</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>1.52587890625E-5</v>
+        <v>6.1035156249944489E-6</v>
       </c>
       <c r="F22" cm="1">
         <f t="array" ref="F22">_xll.XLL.UDF(function,C22)</f>
-        <v>8.3254073523164607E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.9277266237049985E-5</v>
+      </c>
+      <c r="I22" cm="1">
+        <f t="array" ref="I22:J22">_xll.FALSE.POSITIVE(function,I21,J21)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J22">
+        <v>0.16679566610559465</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>6.6795666105594648E-2</v>
+      </c>
+      <c r="L22" cm="1">
+        <f t="array" ref="L22">_xll.XLL.UDF(function,I22)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" cm="1">
         <f t="array" ref="C23:D23">_xll.BISECT(function,C22,D22)</f>
-        <v>1.7577667236328125</v>
+        <v>0.1667938232421875</v>
       </c>
       <c r="D23">
-        <v>1.7577743530273438</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>7.62939453125E-6</v>
+        <v>3.0517578125111022E-6</v>
       </c>
       <c r="F23" cm="1">
         <f t="array" ref="F23">_xll.XLL.UDF(function,C23)</f>
-        <v>8.3254073523164607E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.1022993468123804E-5</v>
+      </c>
+      <c r="I23" cm="1">
+        <f t="array" ref="I23:J23">_xll.FALSE.POSITIVE(function,I22,J22)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J23">
+        <v>0.16679566610011887</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>6.6795666100118861E-2</v>
+      </c>
+      <c r="L23" cm="1">
+        <f t="array" ref="L23">_xll.XLL.UDF(function,I23)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" cm="1">
         <f t="array" ref="C24:D24">_xll.BISECT(function,C23,D23)</f>
-        <v>1.7577705383300781</v>
+        <v>0.16679534912109376</v>
       </c>
       <c r="D24">
-        <v>1.7577743530273438</v>
+        <v>0.16679687500000001</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>3.814697265625E-6</v>
+        <v>1.5258789062555511E-6</v>
       </c>
       <c r="F24" cm="1">
         <f t="array" ref="F24">_xll.XLL.UDF(function,C24)</f>
-        <v>2.3270757298021749E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.8959832049153466E-6</v>
+      </c>
+      <c r="I24" cm="1">
+        <f t="array" ref="I24:J24">_xll.FALSE.POSITIVE(function,I23,J23)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J24">
+        <v>0.16679566609892446</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>6.6795666098924456E-2</v>
+      </c>
+      <c r="L24" cm="1">
+        <f t="array" ref="L24">_xll.XLL.UDF(function,I24)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" cm="1">
         <f t="array" ref="C25:D25">_xll.BISECT(function,C24,D24)</f>
-        <v>1.7577705383300781</v>
+        <v>0.16679534912109376</v>
       </c>
       <c r="D25">
-        <v>1.7577724456787109</v>
+        <v>0.1667961120605469</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>1.9073486328125E-6</v>
+        <v>7.6293945314165335E-7</v>
       </c>
       <c r="F25" cm="1">
         <f t="array" ref="F25">_xll.XLL.UDF(function,C25)</f>
-        <v>2.3270757298021749E-5</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.8959832049153466E-6</v>
+      </c>
+      <c r="I25" cm="1">
+        <f t="array" ref="I25:J25">_xll.FALSE.POSITIVE(function,I24,J24)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J25">
+        <v>0.16679566609866392</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>6.6795666098663914E-2</v>
+      </c>
+      <c r="L25" cm="1">
+        <f t="array" ref="L25">_xll.XLL.UDF(function,I25)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C26" cm="1">
         <f t="array" ref="C26:D26">_xll.BISECT(function,C25,D25)</f>
-        <v>1.7577714920043945</v>
+        <v>0.16679534912109376</v>
       </c>
       <c r="D26">
-        <v>1.7577724456787109</v>
+        <v>0.16679573059082031</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>9.5367431640625E-7</v>
+        <v>3.8146972655694888E-7</v>
       </c>
       <c r="F26" cm="1">
         <f t="array" ref="F26">_xll.XLL.UDF(function,C26)</f>
-        <v>8.2748439389490613E-6</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.8959832049153466E-6</v>
+      </c>
+      <c r="I26" cm="1">
+        <f t="array" ref="I26:J26">_xll.FALSE.POSITIVE(function,I25,J25)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J26">
+        <v>0.16679566609860713</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>6.6795666098607126E-2</v>
+      </c>
+      <c r="L26" cm="1">
+        <f t="array" ref="L26">_xll.XLL.UDF(function,I26)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27" cm="1">
         <f t="array" ref="C27:D27">_xll.BISECT(function,C26,D26)</f>
-        <v>1.7577719688415527</v>
+        <v>0.16679553985595702</v>
       </c>
       <c r="D27">
-        <v>1.7577724456787109</v>
+        <v>0.16679573059082031</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>4.76837158203125E-7</v>
+        <v>1.9073486329235223E-7</v>
       </c>
       <c r="F27" cm="1">
         <f t="array" ref="F27">_xll.XLL.UDF(function,C27)</f>
-        <v>7.7687461441655614E-7</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-7.5511283414221413E-7</v>
+      </c>
+      <c r="I27" cm="1">
+        <f t="array" ref="I27:J27">_xll.FALSE.POSITIVE(function,I26,J26)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J27">
+        <v>0.16679566609859475</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>6.6795666098594747E-2</v>
+      </c>
+      <c r="L27" cm="1">
+        <f t="array" ref="L27">_xll.XLL.UDF(function,I27)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28" cm="1">
         <f t="array" ref="C28:D28">_xll.BISECT(function,C27,D27)</f>
-        <v>1.7577719688415527</v>
+        <v>0.16679563522338867</v>
       </c>
       <c r="D28">
-        <v>1.7577722072601318</v>
+        <v>0.16679573059082031</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>2.384185791015625E-7</v>
+        <v>9.5367431646176115E-8</v>
       </c>
       <c r="F28" cm="1">
         <f t="array" ref="F28">_xll.XLL.UDF(function,C28)</f>
-        <v>7.7687461441655614E-7</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.8467814117959842E-7</v>
+      </c>
+      <c r="I28" cm="1">
+        <f t="array" ref="I28:J28">_xll.FALSE.POSITIVE(function,I27,J27)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J28">
+        <v>0.16679566609859203</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>6.6795666098592027E-2</v>
+      </c>
+      <c r="L28" cm="1">
+        <f t="array" ref="L28">_xll.XLL.UDF(function,I28)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C29" cm="1">
         <f t="array" ref="C29:D29">_xll.BISECT(function,C28,D28)</f>
-        <v>1.7577719688415527</v>
+        <v>0.16679563522338867</v>
       </c>
       <c r="D29">
-        <v>1.7577720880508423</v>
+        <v>0.1667956829071045</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>1.1920928955078125E-7</v>
+        <v>4.7683715836965845E-8</v>
       </c>
       <c r="F29" cm="1">
         <f t="array" ref="F29">_xll.XLL.UDF(function,C29)</f>
-        <v>7.7687461441655614E-7</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.8467814117959842E-7</v>
+      </c>
+      <c r="I29" cm="1">
+        <f t="array" ref="I29:J29">_xll.FALSE.POSITIVE(function,I28,J28)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J29">
+        <v>0.16679566609859145</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>6.6795666098591444E-2</v>
+      </c>
+      <c r="L29" cm="1">
+        <f t="array" ref="L29">_xll.XLL.UDF(function,I29)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C30" cm="1">
         <f t="array" ref="C30:D30">_xll.BISECT(function,C29,D29)</f>
-        <v>1.7577719688415527</v>
+        <v>0.16679565906524657</v>
       </c>
       <c r="D30">
-        <v>1.7577720284461975</v>
+        <v>0.1667956829071045</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>5.9604644775390625E-8</v>
+        <v>2.384185793236071E-8</v>
       </c>
       <c r="F30" cm="1">
         <f t="array" ref="F30">_xll.XLL.UDF(function,C30)</f>
-        <v>7.7687461441655614E-7</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-4.2069519309370162E-8</v>
+      </c>
+      <c r="I30" cm="1">
+        <f t="array" ref="I30:J30">_xll.FALSE.POSITIVE(function,I29,J29)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J30">
+        <v>0.16679566609859131</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>6.6795666098591305E-2</v>
+      </c>
+      <c r="L30" cm="1">
+        <f t="array" ref="L30">_xll.XLL.UDF(function,I30)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C31" cm="1">
         <f t="array" ref="C31:D31">_xll.BISECT(function,C30,D30)</f>
-        <v>1.7577719986438751</v>
+        <v>0.16679565906524657</v>
       </c>
       <c r="D31">
-        <v>1.7577720284461975</v>
+        <v>0.16679567098617554</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>2.9802322387695313E-8</v>
+        <v>1.1920928966180355E-8</v>
       </c>
       <c r="F31" cm="1">
         <f t="array" ref="F31">_xll.XLL.UDF(function,C31)</f>
-        <v>3.0825125207911697E-7</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-4.2069519309370162E-8</v>
+      </c>
+      <c r="I31" cm="1">
+        <f t="array" ref="I31:J31">_xll.FALSE.POSITIVE(function,I30,J30)</f>
+        <v>0.1</v>
+      </c>
+      <c r="J31">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>6.6795666098591278E-2</v>
+      </c>
+      <c r="L31" cm="1">
+        <f t="array" ref="L31">_xll.XLL.UDF(function,I31)</f>
+        <v>-0.51099230432308951</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C32" cm="1">
         <f t="array" ref="C32:D32">_xll.BISECT(function,C31,D31)</f>
-        <v>1.7577720135450363</v>
+        <v>0.16679566502571105</v>
       </c>
       <c r="D32">
-        <v>1.7577720284461975</v>
+        <v>0.16679567098617554</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
-        <v>1.4901161193847656E-8</v>
+        <v>5.9604644830901776E-9</v>
       </c>
       <c r="F32" cm="1">
         <f t="array" ref="F32">_xll.XLL.UDF(function,C32)</f>
-        <v>7.3939558475899503E-8</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-6.4173669917477683E-9</v>
+      </c>
+      <c r="I32" cm="1">
+        <f t="array" ref="I32:J32">_xll.FALSE.POSITIVE(function,I31,J31)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J32">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L32" cm="1">
+        <f t="array" ref="L32">_xll.XLL.UDF(function,I32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C33" cm="1">
         <f t="array" ref="C33:D33">_xll.BISECT(function,C32,D32)</f>
-        <v>1.7577720135450363</v>
+        <v>0.16679566502571105</v>
       </c>
       <c r="D33">
-        <v>1.7577720209956169</v>
+        <v>0.16679566800594331</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>7.4505805969238281E-9</v>
+        <v>2.9802322554228766E-9</v>
       </c>
       <c r="F33" cm="1">
         <f t="array" ref="F33">_xll.XLL.UDF(function,C33)</f>
-        <v>7.3939558475899503E-8</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-6.4173669917477683E-9</v>
+      </c>
+      <c r="I33" cm="1">
+        <f t="array" ref="I33:J33">_xll.FALSE.POSITIVE(function,I32,J32)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J33">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L33" cm="1">
+        <f t="array" ref="L33">_xll.XLL.UDF(function,I33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C34" cm="1">
         <f t="array" ref="C34:D34">_xll.BISECT(function,C33,D33)</f>
-        <v>1.7577720172703266</v>
+        <v>0.16679566502571105</v>
       </c>
       <c r="D34">
-        <v>1.7577720209956169</v>
+        <v>0.16679566651582717</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>3.7252902984619141E-9</v>
+        <v>1.4901161138336505E-9</v>
       </c>
       <c r="F34" cm="1">
         <f t="array" ref="F34">_xll.XLL.UDF(function,C34)</f>
-        <v>1.5361633742827507E-8</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-6.4173669917477683E-9</v>
+      </c>
+      <c r="I34" cm="1">
+        <f t="array" ref="I34:J34">_xll.FALSE.POSITIVE(function,I33,J33)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J34">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L34" cm="1">
+        <f t="array" ref="L34">_xll.XLL.UDF(function,I34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C35" cm="1">
         <f t="array" ref="C35:D35">_xll.BISECT(function,C34,D34)</f>
-        <v>1.7577720172703266</v>
+        <v>0.1667956657707691</v>
       </c>
       <c r="D35">
-        <v>1.7577720191329718</v>
+        <v>0.16679566651582717</v>
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
-        <v>1.862645149230957E-9</v>
+        <v>7.4505807079461306E-10</v>
       </c>
       <c r="F35" cm="1">
         <f t="array" ref="F35">_xll.XLL.UDF(function,C35)</f>
-        <v>1.5361633742827507E-8</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.9608480414174958E-9</v>
+      </c>
+      <c r="I35" cm="1">
+        <f t="array" ref="I35:J35">_xll.FALSE.POSITIVE(function,I34,J34)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J35">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L35" cm="1">
+        <f t="array" ref="L35">_xll.XLL.UDF(function,I35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C36" cm="1">
         <f t="array" ref="C36:D36">_xll.BISECT(function,C35,D35)</f>
-        <v>1.7577720182016492</v>
+        <v>0.1667956657707691</v>
       </c>
       <c r="D36">
-        <v>1.7577720191329718</v>
+        <v>0.16679566614329813</v>
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
-        <v>9.3132257461547852E-10</v>
+        <v>3.7252903539730653E-10</v>
       </c>
       <c r="F36" cm="1">
         <f t="array" ref="F36">_xll.XLL.UDF(function,C36)</f>
-        <v>7.1715255955950852E-10</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.9608480414174958E-9</v>
+      </c>
+      <c r="I36" cm="1">
+        <f t="array" ref="I36:J36">_xll.FALSE.POSITIVE(function,I35,J35)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J36">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" cm="1">
+        <f t="array" ref="L36">_xll.XLL.UDF(function,I36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C37" cm="1">
         <f t="array" ref="C37:D37">_xll.BISECT(function,C36,D36)</f>
-        <v>1.7577720182016492</v>
+        <v>0.1667956659570336</v>
       </c>
       <c r="D37">
-        <v>1.7577720186673105</v>
+        <v>0.16679566614329813</v>
       </c>
       <c r="E37">
         <f t="shared" si="0"/>
-        <v>4.6566128730773926E-10</v>
+        <v>1.8626453157644107E-10</v>
       </c>
       <c r="F37" cm="1">
         <f t="array" ref="F37">_xll.XLL.UDF(function,C37)</f>
-        <v>7.1715255955950852E-10</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-8.4671825142698924E-10</v>
+      </c>
+      <c r="I37" cm="1">
+        <f t="array" ref="I37:J37">_xll.FALSE.POSITIVE(function,I36,J36)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J37">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L37" cm="1">
+        <f t="array" ref="L37">_xll.XLL.UDF(function,I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C38" cm="1">
         <f t="array" ref="C38:D38">_xll.BISECT(function,C37,D37)</f>
-        <v>1.7577720182016492</v>
+        <v>0.16679566605016588</v>
       </c>
       <c r="D38">
-        <v>1.7577720184344798</v>
+        <v>0.16679566614329813</v>
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
-        <v>2.3283064365386963E-10</v>
+        <v>9.3132251910432728E-11</v>
       </c>
       <c r="F38" cm="1">
         <f t="array" ref="F38">_xll.XLL.UDF(function,C38)</f>
-        <v>7.1715255955950852E-10</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.8965352343067166E-10</v>
+      </c>
+      <c r="I38" cm="1">
+        <f t="array" ref="I38:J38">_xll.FALSE.POSITIVE(function,I37,J37)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J38">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L38" cm="1">
+        <f t="array" ref="L38">_xll.XLL.UDF(function,I38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C39" cm="1">
         <f t="array" ref="C39:D39">_xll.BISECT(function,C38,D38)</f>
-        <v>1.7577720182016492</v>
+        <v>0.16679566609673202</v>
       </c>
       <c r="D39">
-        <v>1.7577720183180645</v>
+        <v>0.16679566614329813</v>
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
-        <v>1.1641532182693481E-10</v>
+        <v>4.6566112077428556E-11</v>
       </c>
       <c r="F39" cm="1">
         <f t="array" ref="F39">_xll.XLL.UDF(function,C39)</f>
-        <v>7.1715255955950852E-10</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.1120881993127105E-11</v>
+      </c>
+      <c r="I39" cm="1">
+        <f t="array" ref="I39:J39">_xll.FALSE.POSITIVE(function,I38,J38)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J39">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L39" cm="1">
+        <f t="array" ref="L39">_xll.XLL.UDF(function,I39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C40" cm="1">
         <f t="array" ref="C40:D40">_xll.BISECT(function,C39,D39)</f>
-        <v>1.7577720182016492</v>
+        <v>0.16679566609673202</v>
       </c>
       <c r="D40">
-        <v>1.7577720182598568</v>
+        <v>0.16679566612001506</v>
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
-        <v>5.8207660913467407E-11</v>
+        <v>2.328304216092647E-11</v>
       </c>
       <c r="F40" cm="1">
         <f t="array" ref="F40">_xll.XLL.UDF(function,C40)</f>
-        <v>7.1715255955950852E-10</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.1120881993127105E-11</v>
+      </c>
+      <c r="I40" cm="1">
+        <f t="array" ref="I40:J40">_xll.FALSE.POSITIVE(function,I39,J39)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J40">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L40" cm="1">
+        <f t="array" ref="L40">_xll.XLL.UDF(function,I40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C41" cm="1">
         <f t="array" ref="C41:D41">_xll.BISECT(function,C40,D40)</f>
-        <v>1.757772018230753</v>
+        <v>0.16679566609673202</v>
       </c>
       <c r="D41">
-        <v>1.7577720182598568</v>
+        <v>0.16679566610837354</v>
       </c>
       <c r="E41">
         <f t="shared" si="0"/>
-        <v>2.9103830456733704E-11</v>
+        <v>1.1641521080463235E-11</v>
       </c>
       <c r="F41" cm="1">
         <f t="array" ref="F41">_xll.XLL.UDF(function,C41)</f>
-        <v>2.5951152338166139E-10</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.1120881993127105E-11</v>
+      </c>
+      <c r="I41" cm="1">
+        <f t="array" ref="I41:J41">_xll.FALSE.POSITIVE(function,I40,J40)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J41">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L41" cm="1">
+        <f t="array" ref="L41">_xll.XLL.UDF(function,I41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C42" cm="1">
         <f t="array" ref="C42:D42">_xll.BISECT(function,C41,D41)</f>
-        <v>1.7577720182453049</v>
+        <v>0.16679566609673202</v>
       </c>
       <c r="D42">
-        <v>1.7577720182598568</v>
+        <v>0.16679566610255278</v>
       </c>
       <c r="E42">
         <f t="shared" si="0"/>
-        <v>1.4551915228366852E-11</v>
+        <v>5.8207605402316176E-12</v>
       </c>
       <c r="F42" cm="1">
         <f t="array" ref="F42">_xll.XLL.UDF(function,C42)</f>
-        <v>3.0691893471157528E-11</v>
-      </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.1120881993127105E-11</v>
+      </c>
+      <c r="I42" cm="1">
+        <f t="array" ref="I42:J42">_xll.FALSE.POSITIVE(function,I41,J41)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J42">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L42" cm="1">
+        <f t="array" ref="L42">_xll.XLL.UDF(function,I42)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C43" cm="1">
         <f t="array" ref="C43:D43">_xll.BISECT(function,C42,D42)</f>
-        <v>1.7577720182453049</v>
+        <v>0.16679566609673202</v>
       </c>
       <c r="D43">
-        <v>1.7577720182525809</v>
+        <v>0.16679566609964241</v>
       </c>
       <c r="E43">
         <f t="shared" si="0"/>
-        <v>7.2759576141834259E-12</v>
+        <v>2.9103941479036166E-12</v>
       </c>
       <c r="F43" cm="1">
         <f t="array" ref="F43">_xll.XLL.UDF(function,C43)</f>
-        <v>3.0691893471157528E-11</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.1120881993127105E-11</v>
+      </c>
+      <c r="I43" cm="1">
+        <f t="array" ref="I43:J43">_xll.FALSE.POSITIVE(function,I42,J42)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J43">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L43" cm="1">
+        <f t="array" ref="L43">_xll.XLL.UDF(function,I43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C44" cm="1">
         <f t="array" ref="C44:D44">_xll.BISECT(function,C43,D43)</f>
-        <v>1.7577720182453049</v>
+        <v>0.16679566609818722</v>
       </c>
       <c r="D44">
-        <v>1.7577720182489429</v>
+        <v>0.16679566609964241</v>
       </c>
       <c r="E44">
         <f t="shared" si="0"/>
-        <v>3.637978807091713E-12</v>
+        <v>1.4551970739518083E-12</v>
       </c>
       <c r="F44" cm="1">
         <f t="array" ref="F44">_xll.XLL.UDF(function,C44)</f>
-        <v>3.0691893471157528E-11</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.4166224577044984E-12</v>
+      </c>
+      <c r="I44" cm="1">
+        <f t="array" ref="I44:J44">_xll.FALSE.POSITIVE(function,I43,J43)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J44">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L44" cm="1">
+        <f t="array" ref="L44">_xll.XLL.UDF(function,I44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C45" cm="1">
         <f t="array" ref="C45:D45">_xll.BISECT(function,C44,D44)</f>
-        <v>1.7577720182471239</v>
+        <v>0.16679566609818722</v>
       </c>
       <c r="D45">
-        <v>1.7577720182489429</v>
+        <v>0.16679566609891483</v>
       </c>
       <c r="E45">
         <f t="shared" si="0"/>
-        <v>1.8189894035458565E-12</v>
+        <v>7.2761241476371197E-13</v>
       </c>
       <c r="F45" cm="1">
         <f t="array" ref="F45">_xll.XLL.UDF(function,C45)</f>
-        <v>2.0889956431346945E-12</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.4166224577044984E-12</v>
+      </c>
+      <c r="I45" cm="1">
+        <f t="array" ref="I45:J45">_xll.FALSE.POSITIVE(function,I44,J44)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J45">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L45" cm="1">
+        <f t="array" ref="L45">_xll.XLL.UDF(function,I45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C46" cm="1">
         <f t="array" ref="C46:D46">_xll.BISECT(function,C45,D45)</f>
-        <v>1.7577720182471239</v>
+        <v>0.16679566609855101</v>
       </c>
       <c r="D46">
-        <v>1.7577720182480334</v>
+        <v>0.16679566609891483</v>
       </c>
       <c r="E46">
         <f t="shared" si="0"/>
-        <v>9.0949470177292824E-13</v>
+        <v>3.638200851696638E-13</v>
       </c>
       <c r="F46" cm="1">
         <f t="array" ref="F46">_xll.XLL.UDF(function,C46)</f>
-        <v>2.0889956431346945E-12</v>
-      </c>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.4069635173876292E-13</v>
+      </c>
+      <c r="I46" cm="1">
+        <f t="array" ref="I46:J46">_xll.FALSE.POSITIVE(function,I45,J45)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J46">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L46" cm="1">
+        <f t="array" ref="L46">_xll.XLL.UDF(function,I46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C47" cm="1">
         <f t="array" ref="C47:D47">_xll.BISECT(function,C46,D46)</f>
-        <v>1.7577720182471239</v>
+        <v>0.16679566609855101</v>
       </c>
       <c r="D47">
-        <v>1.7577720182475787</v>
+        <v>0.16679566609873292</v>
       </c>
       <c r="E47">
         <f t="shared" si="0"/>
-        <v>4.5474735088646412E-13</v>
+        <v>1.819100425848319E-13</v>
       </c>
       <c r="F47" cm="1">
         <f t="array" ref="F47">_xll.XLL.UDF(function,C47)</f>
-        <v>2.0889956431346945E-12</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.4069635173876292E-13</v>
+      </c>
+      <c r="I47" cm="1">
+        <f t="array" ref="I47:J47">_xll.FALSE.POSITIVE(function,I46,J46)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J47">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L47" cm="1">
+        <f t="array" ref="L47">_xll.XLL.UDF(function,I47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C48" cm="1">
         <f t="array" ref="C48:D48">_xll.BISECT(function,C47,D47)</f>
-        <v>1.7577720182471239</v>
+        <v>0.16679566609855101</v>
       </c>
       <c r="D48">
-        <v>1.7577720182473513</v>
+        <v>0.16679566609864196</v>
       </c>
       <c r="E48">
         <f t="shared" si="0"/>
-        <v>2.2737367544323206E-13</v>
+        <v>9.095502129241595E-14</v>
       </c>
       <c r="F48" cm="1">
         <f t="array" ref="F48">_xll.XLL.UDF(function,C48)</f>
-        <v>2.0889956431346945E-12</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.4069635173876292E-13</v>
+      </c>
+      <c r="I48" cm="1">
+        <f t="array" ref="I48:J48">_xll.FALSE.POSITIVE(function,I47,J47)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J48">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L48" cm="1">
+        <f t="array" ref="L48">_xll.XLL.UDF(function,I48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C49" cm="1">
         <f t="array" ref="C49:D49">_xll.BISECT(function,C48,D48)</f>
-        <v>1.7577720182472376</v>
+        <v>0.16679566609855101</v>
       </c>
       <c r="D49">
-        <v>1.7577720182473513</v>
+        <v>0.16679566609859647</v>
       </c>
       <c r="E49">
         <f t="shared" si="0"/>
-        <v>1.1368683772161603E-13</v>
+        <v>4.546363285840016E-14</v>
       </c>
       <c r="F49" cm="1">
         <f t="array" ref="F49">_xll.XLL.UDF(function,C49)</f>
-        <v>3.0198066269804258E-13</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.4069635173876292E-13</v>
+      </c>
+      <c r="I49" cm="1">
+        <f t="array" ref="I49:J49">_xll.FALSE.POSITIVE(function,I48,J48)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J49">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L49" cm="1">
+        <f t="array" ref="L49">_xll.XLL.UDF(function,I49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C50" cm="1">
         <f t="array" ref="C50:D50">_xll.BISECT(function,C49,D49)</f>
-        <v>1.7577720182472376</v>
+        <v>0.16679566609857374</v>
       </c>
       <c r="D50">
-        <v>1.7577720182472945</v>
+        <v>0.16679566609859647</v>
       </c>
       <c r="E50">
         <f t="shared" si="0"/>
-        <v>5.6843418860808015E-14</v>
+        <v>2.273181642920008E-14</v>
       </c>
       <c r="F50" cm="1">
         <f t="array" ref="F50">_xll.XLL.UDF(function,C50)</f>
-        <v>3.0198066269804258E-13</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-1.0480505352462027E-13</v>
+      </c>
+      <c r="I50" cm="1">
+        <f t="array" ref="I50:J50">_xll.FALSE.POSITIVE(function,I49,J49)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J50">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L50" cm="1">
+        <f t="array" ref="L50">_xll.XLL.UDF(function,I50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C51" cm="1">
         <f t="array" ref="C51:D51">_xll.BISECT(function,C50,D50)</f>
-        <v>1.7577720182472376</v>
+        <v>0.16679566609858509</v>
       </c>
       <c r="D51">
-        <v>1.757772018247266</v>
+        <v>0.16679566609859647</v>
       </c>
       <c r="E51">
         <f t="shared" si="0"/>
-        <v>2.8421709430404007E-14</v>
+        <v>1.1379786002407855E-14</v>
       </c>
       <c r="F51" cm="1">
         <f t="array" ref="F51">_xll.XLL.UDF(function,C51)</f>
-        <v>3.0198066269804258E-13</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-3.6859404417555879E-14</v>
+      </c>
+      <c r="I51" cm="1">
+        <f t="array" ref="I51:J51">_xll.FALSE.POSITIVE(function,I50,J50)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J51">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L51" cm="1">
+        <f t="array" ref="L51">_xll.XLL.UDF(function,I51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C52" cm="1">
         <f t="array" ref="C52:D52">_xll.BISECT(function,C51,D51)</f>
-        <v>1.7577720182472518</v>
+        <v>0.16679566609859078</v>
       </c>
       <c r="D52">
-        <v>1.757772018247266</v>
+        <v>0.16679566609859647</v>
       </c>
       <c r="E52">
         <f t="shared" si="0"/>
-        <v>1.4210854715202004E-14</v>
+        <v>5.6898930012039273E-15</v>
       </c>
       <c r="F52" cm="1">
         <f t="array" ref="F52">_xll.XLL.UDF(function,C52)</f>
-        <v>7.815970093361102E-14</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.7755575615628953E-15</v>
+      </c>
+      <c r="I52" cm="1">
+        <f t="array" ref="I52:J52">_xll.FALSE.POSITIVE(function,I51,J51)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J52">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L52" cm="1">
+        <f t="array" ref="L52">_xll.XLL.UDF(function,I52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C53" cm="1">
         <f t="array" ref="C53:D53">_xll.BISECT(function,C52,D52)</f>
-        <v>1.7577720182472518</v>
+        <v>0.16679566609859078</v>
       </c>
       <c r="D53">
-        <v>1.7577720182472589</v>
+        <v>0.16679566609859364</v>
       </c>
       <c r="E53">
         <f t="shared" si="0"/>
-        <v>7.1054273576010019E-15</v>
+        <v>2.8588242884097781E-15</v>
       </c>
       <c r="F53" cm="1">
         <f t="array" ref="F53">_xll.XLL.UDF(function,C53)</f>
-        <v>7.815970093361102E-14</v>
-      </c>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.7755575615628953E-15</v>
+      </c>
+      <c r="I53" cm="1">
+        <f t="array" ref="I53:J53">_xll.FALSE.POSITIVE(function,I52,J52)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J53">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L53" cm="1">
+        <f t="array" ref="L53">_xll.XLL.UDF(function,I53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C54" cm="1">
         <f t="array" ref="C54:D54">_xll.BISECT(function,C53,D53)</f>
-        <v>1.7577720182472554</v>
+        <v>0.16679566609859078</v>
       </c>
       <c r="D54">
-        <v>1.7577720182472589</v>
+        <v>0.1667956660985922</v>
       </c>
       <c r="E54">
         <f t="shared" si="0"/>
-        <v>3.5527136788005009E-15</v>
+        <v>1.4155343563970746E-15</v>
       </c>
       <c r="F54" cm="1">
         <f t="array" ref="F54">_xll.XLL.UDF(function,C54)</f>
-        <v>2.3092638912203256E-14</v>
-      </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.7755575615628953E-15</v>
+      </c>
+      <c r="I54" cm="1">
+        <f t="array" ref="I54:J54">_xll.FALSE.POSITIVE(function,I53,J53)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J54">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L54" cm="1">
+        <f t="array" ref="L54">_xll.XLL.UDF(function,I54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C55" cm="1">
         <f t="array" ref="C55:D55">_xll.BISECT(function,C54,D54)</f>
-        <v>1.7577720182472554</v>
+        <v>0.16679566609859078</v>
       </c>
       <c r="D55">
-        <v>1.7577720182472572</v>
+        <v>0.16679566609859148</v>
       </c>
       <c r="E55">
         <f t="shared" si="0"/>
-        <v>1.7763568394002505E-15</v>
+        <v>6.9388939039072284E-16</v>
       </c>
       <c r="F55" cm="1">
         <f t="array" ref="F55">_xll.XLL.UDF(function,C55)</f>
-        <v>2.3092638912203256E-14</v>
-      </c>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-2.7755575615628953E-15</v>
+      </c>
+      <c r="I55" cm="1">
+        <f t="array" ref="I55:J55">_xll.FALSE.POSITIVE(function,I54,J54)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J55">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L55" cm="1">
+        <f t="array" ref="L55">_xll.XLL.UDF(function,I55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C56" cm="1">
         <f t="array" ref="C56:D56">_xll.BISECT(function,C55,D55)</f>
-        <v>1.7577720182472563</v>
+        <v>0.16679566609859114</v>
       </c>
       <c r="D56">
-        <v>1.7577720182472572</v>
+        <v>0.16679566609859148</v>
       </c>
       <c r="E56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.3306690738754696E-16</v>
       </c>
       <c r="F56" cm="1">
         <f t="array" ref="F56">_xll.XLL.UDF(function,C56)</f>
-        <v>8.8817841970012523E-15</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.45">
+        <v>-7.7715611723760987E-16</v>
+      </c>
+      <c r="I56" cm="1">
+        <f t="array" ref="I56:J56">_xll.FALSE.POSITIVE(function,I55,J55)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J56">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L56" cm="1">
+        <f t="array" ref="L56">_xll.XLL.UDF(function,I56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C57" cm="1">
         <f t="array" ref="C57:D57">_xll.BISECT(function,C56,D56)</f>
-        <v>1.7577720182472567</v>
+        <v>0.16679566609859114</v>
       </c>
       <c r="D57">
-        <v>1.7577720182472572</v>
+        <v>0.16679566609859131</v>
       </c>
       <c r="E57">
         <f t="shared" si="0"/>
@@ -2922,6 +3664,21 @@
       </c>
       <c r="F57" cm="1">
         <f t="array" ref="F57">_xll.XLL.UDF(function,C57)</f>
+        <v>-7.7715611723760987E-16</v>
+      </c>
+      <c r="I57" cm="1">
+        <f t="array" ref="I57:J57">_xll.FALSE.POSITIVE(function,I56,J56)</f>
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="J57">
+        <v>0.16679566609859128</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L57" cm="1">
+        <f t="array" ref="L57">_xll.XLL.UDF(function,I57)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fei Qiu uni: fq2145
</commit_message>
<xml_diff>
--- a/hw3.xlsx
+++ b/hw3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal2222\source\repos\xlladdins\xllfloat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiwq\source\repos\FeiwQiu\xllfloat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EDB811-34F1-462D-A5B0-66E0DF56563B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE161728-1718-4B95-96A5-2D9DDB50F675}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5C1C8244-EF68-49EF-BEC5-ED8ACE692021}"/>
+    <workbookView xWindow="2964" yWindow="1644" windowWidth="20064" windowHeight="10716" xr2:uid="{5C1C8244-EF68-49EF-BEC5-ED8ACE692021}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,14 +35,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -1957,30 +1954,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A2213F5-DEFB-4BA9-A6D0-BFA81AA70A6B}">
-  <dimension ref="B2:Q57"/>
+  <dimension ref="B2:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" customWidth="1"/>
-    <col min="13" max="13" width="3.59765625" customWidth="1"/>
+    <col min="7" max="7" width="3.5546875" customWidth="1"/>
+    <col min="13" max="13" width="3.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" cm="1">
-        <f t="array" ref="C2">_xll.KAHAN.A</f>
-        <v>-1412235196</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="C2" s="4">
+        <f>_xll.KAHAN.A</f>
+        <v>-606011322</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1995,7 +1992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>2</v>
       </c>
@@ -2007,17 +2004,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="N5" cm="1">
         <f t="array" ref="N5">_xll.ARRAY.SET(_xll.ARRAY.INTERVAL($C$3,$C$4,100))</f>
-        <v>-412506</v>
+        <v>452</v>
       </c>
       <c r="O5" cm="1">
         <f t="array" ref="O5">_xll.ARRAY.SET(_xll.ARRAY.APPLY(function,_xll.ARRAY.GET(N5)))</f>
-        <v>-412316</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
+        <v>-287480</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2044,7 +2041,7 @@
       </c>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2066,16 +2063,24 @@
       <c r="H7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I7">
+        <f>_xll.FALSE_POSITION(function,C3,C4)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J7">
+        <f>_xll.FALSE_POSITION(function,C3,C4)</f>
+        <v>1.4444444444444444</v>
+      </c>
       <c r="K7">
         <f>J7-I7</f>
         <v>0</v>
       </c>
       <c r="L7" cm="1">
         <f t="array" ref="L7">_xll.XLL.UDF(function,I7)</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C8" cm="1">
         <f t="array" ref="C8:D8">_xll.BISECT(function,C7,D7)</f>
         <v>1.75</v>
@@ -2091,8 +2096,24 @@
         <f t="array" ref="F8">_xll.XLL.UDF(function,C8)</f>
         <v>0.12109375</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="I8">
+        <f>_xll.FALSE_POSITION(function,I7,J7)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J8">
+        <f>_xll.FALSE_POSITION(function,I7,J7)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8" si="1">J8-I8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" cm="1">
+        <f t="array" ref="L8">_xll.XLL.UDF(function,I8)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C9" cm="1">
         <f t="array" ref="C9:D9">_xll.BISECT(function,C8,D8)</f>
         <v>1.75</v>
@@ -2108,8 +2129,24 @@
         <f t="array" ref="F9">_xll.XLL.UDF(function,C9)</f>
         <v>0.12109375</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="I9">
+        <f>_xll.FALSE_POSITION(function,I8,J8)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J9">
+        <f>_xll.FALSE_POSITION(function,I8,J8)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K72" si="2">J9-I9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" cm="1">
+        <f t="array" ref="L9">_xll.XLL.UDF(function,I9)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C10" cm="1">
         <f t="array" ref="C10:D10">_xll.BISECT(function,C9,D9)</f>
         <v>1.75</v>
@@ -2125,8 +2162,24 @@
         <f t="array" ref="F10">_xll.XLL.UDF(function,C10)</f>
         <v>0.12109375</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="I10">
+        <f>_xll.FALSE_POSITION(function,I9,J9)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J10">
+        <f>_xll.FALSE_POSITION(function,I9,J9)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L10" cm="1">
+        <f t="array" ref="L10">_xll.XLL.UDF(function,I10)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C11" cm="1">
         <f t="array" ref="C11:D11">_xll.BISECT(function,C10,D10)</f>
         <v>1.75</v>
@@ -2142,8 +2195,24 @@
         <f t="array" ref="F11">_xll.XLL.UDF(function,C11)</f>
         <v>0.12109375</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="I11">
+        <f>_xll.FALSE_POSITION(function,I10,J10)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J11">
+        <f>_xll.FALSE_POSITION(function,I10,J10)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L11" cm="1">
+        <f t="array" ref="L11">_xll.XLL.UDF(function,I11)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C12" cm="1">
         <f t="array" ref="C12:D12">_xll.BISECT(function,C11,D11)</f>
         <v>1.75</v>
@@ -2159,8 +2228,24 @@
         <f t="array" ref="F12">_xll.XLL.UDF(function,C12)</f>
         <v>0.12109375</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="I12">
+        <f>_xll.FALSE_POSITION(function,I11,J11)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J12">
+        <f>_xll.FALSE_POSITION(function,I11,J11)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12" cm="1">
+        <f t="array" ref="L12">_xll.XLL.UDF(function,I12)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C13" cm="1">
         <f t="array" ref="C13:D13">_xll.BISECT(function,C12,D12)</f>
         <v>1.75</v>
@@ -2176,8 +2261,24 @@
         <f t="array" ref="F13">_xll.XLL.UDF(function,C13)</f>
         <v>0.12109375</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="I13">
+        <f>_xll.FALSE_POSITION(function,I12,J12)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J13">
+        <f>_xll.FALSE_POSITION(function,I12,J12)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L13" cm="1">
+        <f t="array" ref="L13">_xll.XLL.UDF(function,I13)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C14" cm="1">
         <f t="array" ref="C14:D14">_xll.BISECT(function,C13,D13)</f>
         <v>1.75390625</v>
@@ -2193,8 +2294,24 @@
         <f t="array" ref="F14">_xll.XLL.UDF(function,C14)</f>
         <v>6.0510217910632491E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="I14">
+        <f>_xll.FALSE_POSITION(function,I13,J13)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J14">
+        <f>_xll.FALSE_POSITION(function,I13,J13)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L14" cm="1">
+        <f t="array" ref="L14">_xll.XLL.UDF(function,I14)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C15" cm="1">
         <f t="array" ref="C15:D15">_xll.BISECT(function,C14,D14)</f>
         <v>1.755859375</v>
@@ -2210,8 +2327,24 @@
         <f t="array" ref="F15">_xll.XLL.UDF(function,C15)</f>
         <v>3.0007383538759314E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="I15">
+        <f>_xll.FALSE_POSITION(function,I14,J14)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J15">
+        <f>_xll.FALSE_POSITION(function,I14,J14)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L15" cm="1">
+        <f t="array" ref="L15">_xll.XLL.UDF(function,I15)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C16" cm="1">
         <f t="array" ref="C16:D16">_xll.BISECT(function,C15,D15)</f>
         <v>1.7568359375</v>
@@ -2227,8 +2360,24 @@
         <f t="array" ref="F16">_xll.XLL.UDF(function,C16)</f>
         <v>1.4703062041917292E-2</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I16">
+        <f>_xll.FALSE_POSITION(function,I15,J15)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J16">
+        <f>_xll.FALSE_POSITION(function,I15,J15)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L16" cm="1">
+        <f t="array" ref="L16">_xll.XLL.UDF(function,I16)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" cm="1">
         <f t="array" ref="C17:D17">_xll.BISECT(function,C16,D16)</f>
         <v>1.75732421875</v>
@@ -2244,8 +2393,24 @@
         <f t="array" ref="F17">_xll.XLL.UDF(function,C17)</f>
         <v>7.0376580442257364E-3</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I17">
+        <f>_xll.FALSE_POSITION(function,I16,J16)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J17">
+        <f>_xll.FALSE_POSITION(function,I16,J16)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L17" cm="1">
+        <f t="array" ref="L17">_xll.XLL.UDF(function,I17)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" cm="1">
         <f t="array" ref="C18:D18">_xll.BISECT(function,C17,D17)</f>
         <v>1.757568359375</v>
@@ -2261,8 +2426,24 @@
         <f t="array" ref="F18">_xll.XLL.UDF(function,C18)</f>
         <v>3.2016430855001943E-3</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I18">
+        <f>_xll.FALSE_POSITION(function,I17,J17)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J18">
+        <f>_xll.FALSE_POSITION(function,I17,J17)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L18" cm="1">
+        <f t="array" ref="L18">_xll.XLL.UDF(function,I18)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" cm="1">
         <f t="array" ref="C19:D19">_xll.BISECT(function,C18,D18)</f>
         <v>1.7576904296875</v>
@@ -2278,8 +2459,24 @@
         <f t="array" ref="F19">_xll.XLL.UDF(function,C19)</f>
         <v>1.2828070976524941E-3</v>
       </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I19">
+        <f>_xll.FALSE_POSITION(function,I18,J18)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J19">
+        <f>_xll.FALSE_POSITION(function,I18,J18)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L19" cm="1">
+        <f t="array" ref="L19">_xll.XLL.UDF(function,I19)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" cm="1">
         <f t="array" ref="C20:D20">_xll.BISECT(function,C19,D19)</f>
         <v>1.75775146484375</v>
@@ -2295,8 +2492,24 @@
         <f t="array" ref="F20">_xll.XLL.UDF(function,C20)</f>
         <v>3.2318194303826431E-4</v>
       </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I20">
+        <f>_xll.FALSE_POSITION(function,I19,J19)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J20">
+        <f>_xll.FALSE_POSITION(function,I19,J19)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L20" cm="1">
+        <f t="array" ref="L20">_xll.XLL.UDF(function,I20)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" cm="1">
         <f t="array" ref="C21:D21">_xll.BISECT(function,C20,D20)</f>
         <v>1.75775146484375</v>
@@ -2312,8 +2525,24 @@
         <f t="array" ref="F21">_xll.XLL.UDF(function,C21)</f>
         <v>3.2318194303826431E-4</v>
       </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I21">
+        <f>_xll.FALSE_POSITION(function,I20,J20)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J21">
+        <f>_xll.FALSE_POSITION(function,I20,J20)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L21" cm="1">
+        <f t="array" ref="L21">_xll.XLL.UDF(function,I21)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" cm="1">
         <f t="array" ref="C22:D22">_xll.BISECT(function,C21,D21)</f>
         <v>1.7577667236328125</v>
@@ -2329,8 +2558,24 @@
         <f t="array" ref="F22">_xll.XLL.UDF(function,C22)</f>
         <v>8.3254073523164607E-5</v>
       </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I22">
+        <f>_xll.FALSE_POSITION(function,I21,J21)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J22">
+        <f>_xll.FALSE_POSITION(function,I21,J21)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L22" cm="1">
+        <f t="array" ref="L22">_xll.XLL.UDF(function,I22)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" cm="1">
         <f t="array" ref="C23:D23">_xll.BISECT(function,C22,D22)</f>
         <v>1.7577667236328125</v>
@@ -2346,8 +2591,24 @@
         <f t="array" ref="F23">_xll.XLL.UDF(function,C23)</f>
         <v>8.3254073523164607E-5</v>
       </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I23">
+        <f>_xll.FALSE_POSITION(function,I22,J22)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J23">
+        <f>_xll.FALSE_POSITION(function,I22,J22)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L23" cm="1">
+        <f t="array" ref="L23">_xll.XLL.UDF(function,I23)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" cm="1">
         <f t="array" ref="C24:D24">_xll.BISECT(function,C23,D23)</f>
         <v>1.7577705383300781</v>
@@ -2363,8 +2624,24 @@
         <f t="array" ref="F24">_xll.XLL.UDF(function,C24)</f>
         <v>2.3270757298021749E-5</v>
       </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I24">
+        <f>_xll.FALSE_POSITION(function,I23,J23)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J24">
+        <f>_xll.FALSE_POSITION(function,I23,J23)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L24" cm="1">
+        <f t="array" ref="L24">_xll.XLL.UDF(function,I24)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" cm="1">
         <f t="array" ref="C25:D25">_xll.BISECT(function,C24,D24)</f>
         <v>1.7577705383300781</v>
@@ -2380,8 +2657,24 @@
         <f t="array" ref="F25">_xll.XLL.UDF(function,C25)</f>
         <v>2.3270757298021749E-5</v>
       </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I25">
+        <f>_xll.FALSE_POSITION(function,I24,J24)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J25">
+        <f>_xll.FALSE_POSITION(function,I24,J24)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L25" cm="1">
+        <f t="array" ref="L25">_xll.XLL.UDF(function,I25)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C26" cm="1">
         <f t="array" ref="C26:D26">_xll.BISECT(function,C25,D25)</f>
         <v>1.7577714920043945</v>
@@ -2397,8 +2690,24 @@
         <f t="array" ref="F26">_xll.XLL.UDF(function,C26)</f>
         <v>8.2748439389490613E-6</v>
       </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I26">
+        <f>_xll.FALSE_POSITION(function,I25,J25)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J26">
+        <f>_xll.FALSE_POSITION(function,I25,J25)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L26" cm="1">
+        <f t="array" ref="L26">_xll.XLL.UDF(function,I26)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27" cm="1">
         <f t="array" ref="C27:D27">_xll.BISECT(function,C26,D26)</f>
         <v>1.7577719688415527</v>
@@ -2414,8 +2723,24 @@
         <f t="array" ref="F27">_xll.XLL.UDF(function,C27)</f>
         <v>7.7687461441655614E-7</v>
       </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I27">
+        <f>_xll.FALSE_POSITION(function,I26,J26)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J27">
+        <f>_xll.FALSE_POSITION(function,I26,J26)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L27" cm="1">
+        <f t="array" ref="L27">_xll.XLL.UDF(function,I27)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28" cm="1">
         <f t="array" ref="C28:D28">_xll.BISECT(function,C27,D27)</f>
         <v>1.7577719688415527</v>
@@ -2431,8 +2756,24 @@
         <f t="array" ref="F28">_xll.XLL.UDF(function,C28)</f>
         <v>7.7687461441655614E-7</v>
       </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I28">
+        <f>_xll.FALSE_POSITION(function,I27,J27)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J28">
+        <f>_xll.FALSE_POSITION(function,I27,J27)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L28" cm="1">
+        <f t="array" ref="L28">_xll.XLL.UDF(function,I28)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C29" cm="1">
         <f t="array" ref="C29:D29">_xll.BISECT(function,C28,D28)</f>
         <v>1.7577719688415527</v>
@@ -2448,8 +2789,24 @@
         <f t="array" ref="F29">_xll.XLL.UDF(function,C29)</f>
         <v>7.7687461441655614E-7</v>
       </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I29">
+        <f>_xll.FALSE_POSITION(function,I28,J28)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J29">
+        <f>_xll.FALSE_POSITION(function,I28,J28)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L29" cm="1">
+        <f t="array" ref="L29">_xll.XLL.UDF(function,I29)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C30" cm="1">
         <f t="array" ref="C30:D30">_xll.BISECT(function,C29,D29)</f>
         <v>1.7577719688415527</v>
@@ -2465,8 +2822,24 @@
         <f t="array" ref="F30">_xll.XLL.UDF(function,C30)</f>
         <v>7.7687461441655614E-7</v>
       </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I30">
+        <f>_xll.FALSE_POSITION(function,I29,J29)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J30">
+        <f>_xll.FALSE_POSITION(function,I29,J29)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L30" cm="1">
+        <f t="array" ref="L30">_xll.XLL.UDF(function,I30)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C31" cm="1">
         <f t="array" ref="C31:D31">_xll.BISECT(function,C30,D30)</f>
         <v>1.7577719986438751</v>
@@ -2482,8 +2855,24 @@
         <f t="array" ref="F31">_xll.XLL.UDF(function,C31)</f>
         <v>3.0825125207911697E-7</v>
       </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I31">
+        <f>_xll.FALSE_POSITION(function,I30,J30)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J31">
+        <f>_xll.FALSE_POSITION(function,I30,J30)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L31" cm="1">
+        <f t="array" ref="L31">_xll.XLL.UDF(function,I31)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C32" cm="1">
         <f t="array" ref="C32:D32">_xll.BISECT(function,C31,D31)</f>
         <v>1.7577720135450363</v>
@@ -2499,8 +2888,24 @@
         <f t="array" ref="F32">_xll.XLL.UDF(function,C32)</f>
         <v>7.3939558475899503E-8</v>
       </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I32">
+        <f>_xll.FALSE_POSITION(function,I31,J31)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J32">
+        <f>_xll.FALSE_POSITION(function,I31,J31)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L32" cm="1">
+        <f t="array" ref="L32">_xll.XLL.UDF(function,I32)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C33" cm="1">
         <f t="array" ref="C33:D33">_xll.BISECT(function,C32,D32)</f>
         <v>1.7577720135450363</v>
@@ -2516,8 +2921,24 @@
         <f t="array" ref="F33">_xll.XLL.UDF(function,C33)</f>
         <v>7.3939558475899503E-8</v>
       </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I33">
+        <f>_xll.FALSE_POSITION(function,I32,J32)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J33">
+        <f>_xll.FALSE_POSITION(function,I32,J32)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L33" cm="1">
+        <f t="array" ref="L33">_xll.XLL.UDF(function,I33)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C34" cm="1">
         <f t="array" ref="C34:D34">_xll.BISECT(function,C33,D33)</f>
         <v>1.7577720172703266</v>
@@ -2533,8 +2954,24 @@
         <f t="array" ref="F34">_xll.XLL.UDF(function,C34)</f>
         <v>1.5361633742827507E-8</v>
       </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I34">
+        <f>_xll.FALSE_POSITION(function,I33,J33)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J34">
+        <f>_xll.FALSE_POSITION(function,I33,J33)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L34" cm="1">
+        <f t="array" ref="L34">_xll.XLL.UDF(function,I34)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C35" cm="1">
         <f t="array" ref="C35:D35">_xll.BISECT(function,C34,D34)</f>
         <v>1.7577720172703266</v>
@@ -2550,8 +2987,24 @@
         <f t="array" ref="F35">_xll.XLL.UDF(function,C35)</f>
         <v>1.5361633742827507E-8</v>
       </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I35">
+        <f>_xll.FALSE_POSITION(function,I34,J34)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J35">
+        <f>_xll.FALSE_POSITION(function,I34,J34)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L35" cm="1">
+        <f t="array" ref="L35">_xll.XLL.UDF(function,I35)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C36" cm="1">
         <f t="array" ref="C36:D36">_xll.BISECT(function,C35,D35)</f>
         <v>1.7577720182016492</v>
@@ -2567,8 +3020,24 @@
         <f t="array" ref="F36">_xll.XLL.UDF(function,C36)</f>
         <v>7.1715255955950852E-10</v>
       </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I36">
+        <f>_xll.FALSE_POSITION(function,I35,J35)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J36">
+        <f>_xll.FALSE_POSITION(function,I35,J35)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L36" cm="1">
+        <f t="array" ref="L36">_xll.XLL.UDF(function,I36)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C37" cm="1">
         <f t="array" ref="C37:D37">_xll.BISECT(function,C36,D36)</f>
         <v>1.7577720182016492</v>
@@ -2584,8 +3053,24 @@
         <f t="array" ref="F37">_xll.XLL.UDF(function,C37)</f>
         <v>7.1715255955950852E-10</v>
       </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I37">
+        <f>_xll.FALSE_POSITION(function,I36,J36)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J37">
+        <f>_xll.FALSE_POSITION(function,I36,J36)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L37" cm="1">
+        <f t="array" ref="L37">_xll.XLL.UDF(function,I37)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C38" cm="1">
         <f t="array" ref="C38:D38">_xll.BISECT(function,C37,D37)</f>
         <v>1.7577720182016492</v>
@@ -2601,8 +3086,24 @@
         <f t="array" ref="F38">_xll.XLL.UDF(function,C38)</f>
         <v>7.1715255955950852E-10</v>
       </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I38">
+        <f>_xll.FALSE_POSITION(function,I37,J37)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J38">
+        <f>_xll.FALSE_POSITION(function,I37,J37)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L38" cm="1">
+        <f t="array" ref="L38">_xll.XLL.UDF(function,I38)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C39" cm="1">
         <f t="array" ref="C39:D39">_xll.BISECT(function,C38,D38)</f>
         <v>1.7577720182016492</v>
@@ -2618,8 +3119,24 @@
         <f t="array" ref="F39">_xll.XLL.UDF(function,C39)</f>
         <v>7.1715255955950852E-10</v>
       </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I39">
+        <f>_xll.FALSE_POSITION(function,I38,J38)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J39">
+        <f>_xll.FALSE_POSITION(function,I38,J38)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L39" cm="1">
+        <f t="array" ref="L39">_xll.XLL.UDF(function,I39)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C40" cm="1">
         <f t="array" ref="C40:D40">_xll.BISECT(function,C39,D39)</f>
         <v>1.7577720182016492</v>
@@ -2635,8 +3152,24 @@
         <f t="array" ref="F40">_xll.XLL.UDF(function,C40)</f>
         <v>7.1715255955950852E-10</v>
       </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I40">
+        <f>_xll.FALSE_POSITION(function,I39,J39)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J40">
+        <f>_xll.FALSE_POSITION(function,I39,J39)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L40" cm="1">
+        <f t="array" ref="L40">_xll.XLL.UDF(function,I40)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C41" cm="1">
         <f t="array" ref="C41:D41">_xll.BISECT(function,C40,D40)</f>
         <v>1.757772018230753</v>
@@ -2652,8 +3185,24 @@
         <f t="array" ref="F41">_xll.XLL.UDF(function,C41)</f>
         <v>2.5951152338166139E-10</v>
       </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I41">
+        <f>_xll.FALSE_POSITION(function,I40,J40)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J41">
+        <f>_xll.FALSE_POSITION(function,I40,J40)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L41" cm="1">
+        <f t="array" ref="L41">_xll.XLL.UDF(function,I41)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C42" cm="1">
         <f t="array" ref="C42:D42">_xll.BISECT(function,C41,D41)</f>
         <v>1.7577720182453049</v>
@@ -2669,8 +3218,24 @@
         <f t="array" ref="F42">_xll.XLL.UDF(function,C42)</f>
         <v>3.0691893471157528E-11</v>
       </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I42">
+        <f>_xll.FALSE_POSITION(function,I41,J41)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J42">
+        <f>_xll.FALSE_POSITION(function,I41,J41)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L42" cm="1">
+        <f t="array" ref="L42">_xll.XLL.UDF(function,I42)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C43" cm="1">
         <f t="array" ref="C43:D43">_xll.BISECT(function,C42,D42)</f>
         <v>1.7577720182453049</v>
@@ -2686,8 +3251,24 @@
         <f t="array" ref="F43">_xll.XLL.UDF(function,C43)</f>
         <v>3.0691893471157528E-11</v>
       </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I43">
+        <f>_xll.FALSE_POSITION(function,I42,J42)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J43">
+        <f>_xll.FALSE_POSITION(function,I42,J42)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L43" cm="1">
+        <f t="array" ref="L43">_xll.XLL.UDF(function,I43)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C44" cm="1">
         <f t="array" ref="C44:D44">_xll.BISECT(function,C43,D43)</f>
         <v>1.7577720182453049</v>
@@ -2703,8 +3284,24 @@
         <f t="array" ref="F44">_xll.XLL.UDF(function,C44)</f>
         <v>3.0691893471157528E-11</v>
       </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I44">
+        <f>_xll.FALSE_POSITION(function,I43,J43)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J44">
+        <f>_xll.FALSE_POSITION(function,I43,J43)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L44" cm="1">
+        <f t="array" ref="L44">_xll.XLL.UDF(function,I44)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C45" cm="1">
         <f t="array" ref="C45:D45">_xll.BISECT(function,C44,D44)</f>
         <v>1.7577720182471239</v>
@@ -2720,8 +3317,24 @@
         <f t="array" ref="F45">_xll.XLL.UDF(function,C45)</f>
         <v>2.0889956431346945E-12</v>
       </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I45">
+        <f>_xll.FALSE_POSITION(function,I44,J44)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J45">
+        <f>_xll.FALSE_POSITION(function,I44,J44)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L45" cm="1">
+        <f t="array" ref="L45">_xll.XLL.UDF(function,I45)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C46" cm="1">
         <f t="array" ref="C46:D46">_xll.BISECT(function,C45,D45)</f>
         <v>1.7577720182471239</v>
@@ -2737,8 +3350,24 @@
         <f t="array" ref="F46">_xll.XLL.UDF(function,C46)</f>
         <v>2.0889956431346945E-12</v>
       </c>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I46">
+        <f>_xll.FALSE_POSITION(function,I45,J45)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J46">
+        <f>_xll.FALSE_POSITION(function,I45,J45)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L46" cm="1">
+        <f t="array" ref="L46">_xll.XLL.UDF(function,I46)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C47" cm="1">
         <f t="array" ref="C47:D47">_xll.BISECT(function,C46,D46)</f>
         <v>1.7577720182471239</v>
@@ -2754,8 +3383,24 @@
         <f t="array" ref="F47">_xll.XLL.UDF(function,C47)</f>
         <v>2.0889956431346945E-12</v>
       </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I47">
+        <f>_xll.FALSE_POSITION(function,I46,J46)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J47">
+        <f>_xll.FALSE_POSITION(function,I46,J46)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L47" cm="1">
+        <f t="array" ref="L47">_xll.XLL.UDF(function,I47)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C48" cm="1">
         <f t="array" ref="C48:D48">_xll.BISECT(function,C47,D47)</f>
         <v>1.7577720182471239</v>
@@ -2771,8 +3416,24 @@
         <f t="array" ref="F48">_xll.XLL.UDF(function,C48)</f>
         <v>2.0889956431346945E-12</v>
       </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I48">
+        <f>_xll.FALSE_POSITION(function,I47,J47)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J48">
+        <f>_xll.FALSE_POSITION(function,I47,J47)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L48" cm="1">
+        <f t="array" ref="L48">_xll.XLL.UDF(function,I48)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C49" cm="1">
         <f t="array" ref="C49:D49">_xll.BISECT(function,C48,D48)</f>
         <v>1.7577720182472376</v>
@@ -2788,8 +3449,24 @@
         <f t="array" ref="F49">_xll.XLL.UDF(function,C49)</f>
         <v>3.0198066269804258E-13</v>
       </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I49">
+        <f>_xll.FALSE_POSITION(function,I48,J48)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J49">
+        <f>_xll.FALSE_POSITION(function,I48,J48)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L49" cm="1">
+        <f t="array" ref="L49">_xll.XLL.UDF(function,I49)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C50" cm="1">
         <f t="array" ref="C50:D50">_xll.BISECT(function,C49,D49)</f>
         <v>1.7577720182472376</v>
@@ -2805,8 +3482,24 @@
         <f t="array" ref="F50">_xll.XLL.UDF(function,C50)</f>
         <v>3.0198066269804258E-13</v>
       </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I50">
+        <f>_xll.FALSE_POSITION(function,I49,J49)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J50">
+        <f>_xll.FALSE_POSITION(function,I49,J49)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L50" cm="1">
+        <f t="array" ref="L50">_xll.XLL.UDF(function,I50)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C51" cm="1">
         <f t="array" ref="C51:D51">_xll.BISECT(function,C50,D50)</f>
         <v>1.7577720182472376</v>
@@ -2822,8 +3515,24 @@
         <f t="array" ref="F51">_xll.XLL.UDF(function,C51)</f>
         <v>3.0198066269804258E-13</v>
       </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I51">
+        <f>_xll.FALSE_POSITION(function,I50,J50)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J51">
+        <f>_xll.FALSE_POSITION(function,I50,J50)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L51" cm="1">
+        <f t="array" ref="L51">_xll.XLL.UDF(function,I51)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C52" cm="1">
         <f t="array" ref="C52:D52">_xll.BISECT(function,C51,D51)</f>
         <v>1.7577720182472518</v>
@@ -2839,8 +3548,24 @@
         <f t="array" ref="F52">_xll.XLL.UDF(function,C52)</f>
         <v>7.815970093361102E-14</v>
       </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I52">
+        <f>_xll.FALSE_POSITION(function,I51,J51)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J52">
+        <f>_xll.FALSE_POSITION(function,I51,J51)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L52" cm="1">
+        <f t="array" ref="L52">_xll.XLL.UDF(function,I52)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C53" cm="1">
         <f t="array" ref="C53:D53">_xll.BISECT(function,C52,D52)</f>
         <v>1.7577720182472518</v>
@@ -2856,8 +3581,24 @@
         <f t="array" ref="F53">_xll.XLL.UDF(function,C53)</f>
         <v>7.815970093361102E-14</v>
       </c>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I53">
+        <f>_xll.FALSE_POSITION(function,I52,J52)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J53">
+        <f>_xll.FALSE_POSITION(function,I52,J52)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L53" cm="1">
+        <f t="array" ref="L53">_xll.XLL.UDF(function,I53)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C54" cm="1">
         <f t="array" ref="C54:D54">_xll.BISECT(function,C53,D53)</f>
         <v>1.7577720182472554</v>
@@ -2873,8 +3614,24 @@
         <f t="array" ref="F54">_xll.XLL.UDF(function,C54)</f>
         <v>2.3092638912203256E-14</v>
       </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I54">
+        <f>_xll.FALSE_POSITION(function,I53,J53)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J54">
+        <f>_xll.FALSE_POSITION(function,I53,J53)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L54" cm="1">
+        <f t="array" ref="L54">_xll.XLL.UDF(function,I54)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C55" cm="1">
         <f t="array" ref="C55:D55">_xll.BISECT(function,C54,D54)</f>
         <v>1.7577720182472554</v>
@@ -2890,8 +3647,24 @@
         <f t="array" ref="F55">_xll.XLL.UDF(function,C55)</f>
         <v>2.3092638912203256E-14</v>
       </c>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I55">
+        <f>_xll.FALSE_POSITION(function,I54,J54)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J55">
+        <f>_xll.FALSE_POSITION(function,I54,J54)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L55" cm="1">
+        <f t="array" ref="L55">_xll.XLL.UDF(function,I55)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C56" cm="1">
         <f t="array" ref="C56:D56">_xll.BISECT(function,C55,D55)</f>
         <v>1.7577720182472563</v>
@@ -2907,8 +3680,24 @@
         <f t="array" ref="F56">_xll.XLL.UDF(function,C56)</f>
         <v>8.8817841970012523E-15</v>
       </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="I56">
+        <f>_xll.FALSE_POSITION(function,I55,J55)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J56">
+        <f>_xll.FALSE_POSITION(function,I55,J55)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L56" cm="1">
+        <f t="array" ref="L56">_xll.XLL.UDF(function,I56)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C57" cm="1">
         <f t="array" ref="C57:D57">_xll.BISECT(function,C56,D56)</f>
         <v>1.7577720182472567</v>
@@ -2923,6 +3712,490 @@
       <c r="F57" cm="1">
         <f t="array" ref="F57">_xll.XLL.UDF(function,C57)</f>
         <v>0</v>
+      </c>
+      <c r="I57">
+        <f>_xll.FALSE_POSITION(function,I56,J56)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J57">
+        <f>_xll.FALSE_POSITION(function,I56,J56)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L57" cm="1">
+        <f t="array" ref="L57">_xll.XLL.UDF(function,I57)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="I58">
+        <f>_xll.FALSE_POSITION(function,I57,J57)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J58">
+        <f>_xll.FALSE_POSITION(function,I57,J57)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L58" cm="1">
+        <f t="array" ref="L58">_xll.XLL.UDF(function,I58)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="59" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="I59">
+        <f>_xll.FALSE_POSITION(function,I58,J58)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J59">
+        <f>_xll.FALSE_POSITION(function,I58,J58)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L59" cm="1">
+        <f t="array" ref="L59">_xll.XLL.UDF(function,I59)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="I60">
+        <f>_xll.FALSE_POSITION(function,I59,J59)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J60">
+        <f>_xll.FALSE_POSITION(function,I59,J59)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L60" cm="1">
+        <f t="array" ref="L60">_xll.XLL.UDF(function,I60)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="I61">
+        <f>_xll.FALSE_POSITION(function,I60,J60)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J61">
+        <f>_xll.FALSE_POSITION(function,I60,J60)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L61" cm="1">
+        <f t="array" ref="L61">_xll.XLL.UDF(function,I61)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="I62">
+        <f>_xll.FALSE_POSITION(function,I61,J61)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J62">
+        <f>_xll.FALSE_POSITION(function,I61,J61)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L62" cm="1">
+        <f t="array" ref="L62">_xll.XLL.UDF(function,I62)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="63" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="I63">
+        <f>_xll.FALSE_POSITION(function,I62,J62)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J63">
+        <f>_xll.FALSE_POSITION(function,I62,J62)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L63" cm="1">
+        <f t="array" ref="L63">_xll.XLL.UDF(function,I63)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="64" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="I64">
+        <f>_xll.FALSE_POSITION(function,I63,J63)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J64">
+        <f>_xll.FALSE_POSITION(function,I63,J63)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L64" cm="1">
+        <f t="array" ref="L64">_xll.XLL.UDF(function,I64)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="65" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I65">
+        <f>_xll.FALSE_POSITION(function,I64,J64)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J65">
+        <f>_xll.FALSE_POSITION(function,I64,J64)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L65" cm="1">
+        <f t="array" ref="L65">_xll.XLL.UDF(function,I65)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="66" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I66">
+        <f>_xll.FALSE_POSITION(function,I65,J65)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J66">
+        <f>_xll.FALSE_POSITION(function,I65,J65)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L66" cm="1">
+        <f t="array" ref="L66">_xll.XLL.UDF(function,I66)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="67" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I67">
+        <f>_xll.FALSE_POSITION(function,I66,J66)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J67">
+        <f>_xll.FALSE_POSITION(function,I66,J66)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L67" cm="1">
+        <f t="array" ref="L67">_xll.XLL.UDF(function,I67)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="68" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I68">
+        <f>_xll.FALSE_POSITION(function,I67,J67)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J68">
+        <f>_xll.FALSE_POSITION(function,I67,J67)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L68" cm="1">
+        <f t="array" ref="L68">_xll.XLL.UDF(function,I68)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="69" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I69">
+        <f>_xll.FALSE_POSITION(function,I68,J68)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J69">
+        <f>_xll.FALSE_POSITION(function,I68,J68)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L69" cm="1">
+        <f t="array" ref="L69">_xll.XLL.UDF(function,I69)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="70" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I70">
+        <f>_xll.FALSE_POSITION(function,I69,J69)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J70">
+        <f>_xll.FALSE_POSITION(function,I69,J69)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L70" cm="1">
+        <f t="array" ref="L70">_xll.XLL.UDF(function,I70)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="71" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I71">
+        <f>_xll.FALSE_POSITION(function,I70,J70)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J71">
+        <f>_xll.FALSE_POSITION(function,I70,J70)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L71" cm="1">
+        <f t="array" ref="L71">_xll.XLL.UDF(function,I71)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="72" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I72">
+        <f>_xll.FALSE_POSITION(function,I71,J71)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J72">
+        <f>_xll.FALSE_POSITION(function,I71,J71)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L72" cm="1">
+        <f t="array" ref="L72">_xll.XLL.UDF(function,I72)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="73" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I73">
+        <f>_xll.FALSE_POSITION(function,I72,J72)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J73">
+        <f>_xll.FALSE_POSITION(function,I72,J72)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K73">
+        <f t="shared" ref="K73:K83" si="3">J73-I73</f>
+        <v>0</v>
+      </c>
+      <c r="L73" cm="1">
+        <f t="array" ref="L73">_xll.XLL.UDF(function,I73)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="74" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I74">
+        <f>_xll.FALSE_POSITION(function,I73,J73)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J74">
+        <f>_xll.FALSE_POSITION(function,I73,J73)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L74" cm="1">
+        <f t="array" ref="L74">_xll.XLL.UDF(function,I74)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="75" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I75">
+        <f>_xll.FALSE_POSITION(function,I74,J74)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J75">
+        <f>_xll.FALSE_POSITION(function,I74,J74)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L75" cm="1">
+        <f t="array" ref="L75">_xll.XLL.UDF(function,I75)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="76" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I76">
+        <f>_xll.FALSE_POSITION(function,I75,J75)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J76">
+        <f>_xll.FALSE_POSITION(function,I75,J75)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L76" cm="1">
+        <f t="array" ref="L76">_xll.XLL.UDF(function,I76)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="77" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I77">
+        <f>_xll.FALSE_POSITION(function,I76,J76)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J77">
+        <f>_xll.FALSE_POSITION(function,I76,J76)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L77" cm="1">
+        <f t="array" ref="L77">_xll.XLL.UDF(function,I77)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="78" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I78">
+        <f>_xll.FALSE_POSITION(function,I77,J77)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J78">
+        <f>_xll.FALSE_POSITION(function,I77,J77)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L78" cm="1">
+        <f t="array" ref="L78">_xll.XLL.UDF(function,I78)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="79" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I79">
+        <f>_xll.FALSE_POSITION(function,I78,J78)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J79">
+        <f>_xll.FALSE_POSITION(function,I78,J78)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L79" cm="1">
+        <f t="array" ref="L79">_xll.XLL.UDF(function,I79)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="80" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I80">
+        <f>_xll.FALSE_POSITION(function,I79,J79)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J80">
+        <f>_xll.FALSE_POSITION(function,I79,J79)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L80" cm="1">
+        <f t="array" ref="L80">_xll.XLL.UDF(function,I80)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="81" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I81">
+        <f>_xll.FALSE_POSITION(function,I80,J80)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J81">
+        <f>_xll.FALSE_POSITION(function,I80,J80)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L81" cm="1">
+        <f t="array" ref="L81">_xll.XLL.UDF(function,I81)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="82" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I82">
+        <f>_xll.FALSE_POSITION(function,I81,J81)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J82">
+        <f>_xll.FALSE_POSITION(function,I81,J81)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L82" cm="1">
+        <f t="array" ref="L82">_xll.XLL.UDF(function,I82)</f>
+        <v>3.31351928059747</v>
+      </c>
+    </row>
+    <row r="83" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I83">
+        <f>_xll.FALSE_POSITION(function,I82,J82)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="J83">
+        <f>_xll.FALSE_POSITION(function,I82,J82)</f>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L83" cm="1">
+        <f t="array" ref="L83">_xll.XLL.UDF(function,I83)</f>
+        <v>3.31351928059747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>